<commit_message>
currency codes, media types, and ad units
</commit_message>
<xml_diff>
--- a/model/schemas/currencyCodes.xlsx
+++ b/model/schemas/currencyCodes.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="360" yWindow="45" windowWidth="19155" windowHeight="9780"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Currency Codes" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="333">
   <si>
     <t>AED</t>
   </si>
@@ -998,13 +998,28 @@
   </si>
   <si>
     <t>Zimbabwe Dollar</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>XSD Enumeration Code</t>
+  </si>
+  <si>
+    <t>ISO 4217 Currency Codes</t>
+  </si>
+  <si>
+    <t>sourced from http://en.wikipedia.org/wiki/ISO_4217</t>
+  </si>
+  <si>
+    <t>Currency Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1012,13 +1027,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1033,8 +1070,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1329,1984 +1368,2007 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C164"/>
+  <dimension ref="A1:C168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="B162" sqref="B162"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="66.5703125" customWidth="1"/>
     <col min="3" max="3" width="78.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="str">
-        <f t="shared" ref="C1:C64" si="0">CONCATENATE("&lt;xs:enumeration value=''",A1,"''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;",B1,"&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;")</f>
-        <v>&lt;xs:enumeration value=''AED''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;United Arab Emirates Dirham&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+    <row r="1" spans="1:3" ht="21">
+      <c r="A1" s="2" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''AFN''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Afghanistan Afghani&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''ALL''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Albania Lek&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''AMD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Armenia Dram&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1">
+      <c r="A4" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''ANG''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Netherlands Antilles Guilder&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <f>CONCATENATE("&lt;xs:enumeration value=""",A5,"""&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;",B5,"&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;")</f>
+        <v>&lt;xs:enumeration value="AED"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;United Arab Emirates Dirham&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''AOA''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Angola Kwanza&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <f t="shared" ref="C6:C69" si="0">CONCATENATE("&lt;xs:enumeration value=""",A6,"""&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;",B6,"&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;")</f>
+        <v>&lt;xs:enumeration value="AFN"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Afghanistan Afghani&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''ARS''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Argentina Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="ALL"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Albania Lek&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''AUD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Australia Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="AMD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Armenia Dram&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''AWG''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Aruba Guilder&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="ANG"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Netherlands Antilles Guilder&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''AZN''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Azerbaijan New Manat&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="AOA"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Angola Kwanza&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''BAM''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bosnia and Herzegovina Convertible Marka&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="ARS"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Argentina Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''BBD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Barbados Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="AUD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Australia Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''BDT''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bangladesh Taka&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="AWG"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Aruba Guilder&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''BGN''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bulgaria Lev&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="AZN"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Azerbaijan New Manat&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''BHD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bahrain Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="BAM"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bosnia and Herzegovina Convertible Marka&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''BIF''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Burundi Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="BBD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Barbados Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''BMD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bermuda Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="BDT"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bangladesh Taka&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''BND''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Brunei Darussalam Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="BGN"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bulgaria Lev&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''BOB''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bolivia Boliviano&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="BHD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bahrain Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''BRL''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Brazil Real&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="BIF"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Burundi Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''BSD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bahamas Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="BMD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bermuda Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''BTN''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bhutan Ngultrum&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="BND"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Brunei Darussalam Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''BWP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Botswana Pula&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="BOB"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bolivia Boliviano&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''BYR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Belarus Ruble&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="BRL"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Brazil Real&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''BZD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Belize Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="BSD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bahamas Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''CAD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Canada Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="BTN"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Bhutan Ngultrum&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''CDF''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Congo/Kinshasa Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="BWP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Botswana Pula&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''CHF''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Switzerland Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="BYR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Belarus Ruble&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''CLP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Chile Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="BZD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Belize Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''CNY''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;China Yuan Renminbi&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="CAD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Canada Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''COP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Colombia Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="CDF"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Congo/Kinshasa Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''CRC''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Costa Rica Colon&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="CHF"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Switzerland Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''CUC''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Cuba Convertible Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="CLP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Chile Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''CUP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Cuba Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="CNY"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;China Yuan Renminbi&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''CVE''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Cape Verde Escudo&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="COP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Colombia Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''CZK''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Czech Republic Koruna&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="CRC"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Costa Rica Colon&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''DJF''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Djibouti Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="CUC"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Cuba Convertible Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''DKK''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Denmark Krone&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="CUP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Cuba Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''DOP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Dominican Republic Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="CVE"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Cape Verde Escudo&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''DZD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Algeria Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="CZK"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Czech Republic Koruna&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''EGP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Egypt Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="DJF"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Djibouti Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''ERN''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Eritrea Nakfa&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="DKK"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Denmark Krone&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''ETB''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Ethiopia Birr&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="DOP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Dominican Republic Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''EUR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Euro Member Countries&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="DZD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Algeria Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''FJD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Fiji Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="EGP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Egypt Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''FKP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Falkland Islands (Malvinas) Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="ERN"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Eritrea Nakfa&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''GBP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;United Kingdom Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="ETB"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Ethiopia Birr&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''GEL''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Georgia Lari&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="EUR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Euro Member Countries&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''GGP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Guernsey Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="FJD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Fiji Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''GHS''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Ghana Cedi&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="FKP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Falkland Islands (Malvinas) Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''GIP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Gibraltar Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="GBP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;United Kingdom Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''GMD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Gambia Dalasi&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="GEL"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Georgia Lari&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''GNF''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Guinea Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="GGP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Guernsey Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''GTQ''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Guatemala Quetzal&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="GHS"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Ghana Cedi&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B55" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''GYD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Guyana Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="GIP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Gibraltar Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B56" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''HKD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Hong Kong Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="GMD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Gambia Dalasi&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''HNL''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Honduras Lempira&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="GNF"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Guinea Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''HRK''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Croatia Kuna&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="GTQ"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Guatemala Quetzal&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''HTG''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Haiti Gourde&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="GYD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Guyana Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''HUF''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Hungary Forint&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="HKD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Hong Kong Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''IDR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Indonesia Rupiah&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="HNL"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Honduras Lempira&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B62" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''ILS''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Israel Shekel&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="HRK"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Croatia Kuna&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B63" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''IMP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Isle of Man Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="HTG"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Haiti Gourde&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;xs:enumeration value=''INR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;India Rupee&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="HUF"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Hungary Forint&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B65" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C65" t="str">
-        <f t="shared" ref="C65:C128" si="1">CONCATENATE("&lt;xs:enumeration value=''",A65,"''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;",B65,"&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;")</f>
-        <v>&lt;xs:enumeration value=''IQD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Iraq Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;xs:enumeration value="IDR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Indonesia Rupiah&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B66" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''IRR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Iran Rial&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;xs:enumeration value="ILS"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Israel Shekel&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B67" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''ISK''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Iceland Krona&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;xs:enumeration value="IMP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Isle of Man Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B68" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C68" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''JEP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Jersey Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;xs:enumeration value="INR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;India Rupee&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B69" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C69" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''JMD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Jamaica Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;xs:enumeration value="IQD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Iraq Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B70" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C70" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''JOD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Jordan Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <f t="shared" ref="C70:C133" si="1">CONCATENATE("&lt;xs:enumeration value=""",A70,"""&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;",B70,"&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;")</f>
+        <v>&lt;xs:enumeration value="IRR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Iran Rial&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B71" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''JPY''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Japan Yen&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="ISK"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Iceland Krona&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B72" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''KES''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Kenya Shilling&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="JEP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Jersey Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B73" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''KGS''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Kyrgyzstan Som&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="JMD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Jamaica Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B74" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''KHR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Cambodia Riel&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="JOD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Jordan Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B75" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''KMF''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Comoros Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="JPY"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Japan Yen&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B76" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''KPW''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Korea (North) Won&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="KES"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Kenya Shilling&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B77" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''KRW''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Korea (South) Won&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="KGS"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Kyrgyzstan Som&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B78" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''KWD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Kuwait Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="KHR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Cambodia Riel&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B79" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''KYD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Cayman Islands Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="KMF"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Comoros Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B80" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''KZT''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Kazakhstan Tenge&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="KPW"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Korea (North) Won&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B81" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''LAK''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Laos Kip&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="KRW"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Korea (South) Won&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B82" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''LBP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Lebanon Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="KWD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Kuwait Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B83" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''LKR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Sri Lanka Rupee&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="KYD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Cayman Islands Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B84" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''LRD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Liberia Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="KZT"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Kazakhstan Tenge&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B85" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''LSL''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Lesotho Loti&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="LAK"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Laos Kip&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B86" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''LTL''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Lithuania Litas&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="LBP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Lebanon Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B87" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''LVL''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Latvia Lat&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="LKR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Sri Lanka Rupee&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B88" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''LYD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Libya Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="LRD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Liberia Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B89" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''MAD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Morocco Dirham&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="LSL"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Lesotho Loti&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B90" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''MDL''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Moldova Leu&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="LTL"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Lithuania Litas&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B91" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''MGA''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Madagascar Ariary&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="LVL"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Latvia Lat&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B92" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''MKD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Macedonia Denar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="LYD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Libya Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B93" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''MMK''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Myanmar (Burma) Kyat&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="MAD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Morocco Dirham&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B94" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''MNT''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Mongolia Tughrik&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="MDL"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Moldova Leu&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B95" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''MOP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Macau Pataca&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="MGA"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Madagascar Ariary&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B96" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''MRO''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Mauritania Ouguiya&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="MKD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Macedonia Denar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B97" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''MUR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Mauritius Rupee&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="MMK"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Myanmar (Burma) Kyat&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B98" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''MVR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Maldives (Maldive Islands) Rufiyaa&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="MNT"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Mongolia Tughrik&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B99" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''MWK''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Malawi Kwacha&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="MOP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Macau Pataca&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B100" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''MXN''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Mexico Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="MRO"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Mauritania Ouguiya&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B101" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''MYR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Malaysia Ringgit&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="MUR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Mauritius Rupee&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B102" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''MZN''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Mozambique Metical&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="MVR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Maldives (Maldive Islands) Rufiyaa&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B103" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''NAD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Namibia Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="MWK"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Malawi Kwacha&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B104" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''NGN''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Nigeria Naira&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="MXN"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Mexico Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B105" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''NIO''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Nicaragua Cordoba&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="MYR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Malaysia Ringgit&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B106" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C106" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''NOK''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Norway Krone&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="MZN"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Mozambique Metical&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B107" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C107" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''NPR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Nepal Rupee&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="NAD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Namibia Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B108" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C108" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''NZD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;New Zealand Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="NGN"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Nigeria Naira&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B109" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="C109" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''OMR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Oman Rial&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="NIO"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Nicaragua Cordoba&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B110" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C110" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''PAB''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Panama Balboa&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="NOK"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Norway Krone&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B111" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C111" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''PEN''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Peru Nuevo Sol&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="NPR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Nepal Rupee&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B112" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="C112" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''PGK''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Papua New Guinea Kina&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="NZD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;New Zealand Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B113" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C113" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''PHP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Philippines Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="OMR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Oman Rial&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B114" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C114" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''PKR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Pakistan Rupee&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="PAB"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Panama Balboa&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B115" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C115" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''PLN''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Poland Zloty&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="PEN"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Peru Nuevo Sol&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B116" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C116" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''PYG''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Paraguay Guarani&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="PGK"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Papua New Guinea Kina&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B117" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C117" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''QAR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Qatar Riyal&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="PHP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Philippines Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B118" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C118" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''RON''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Romania New Leu&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="PKR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Pakistan Rupee&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B119" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C119" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''RSD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Serbia Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="PLN"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Poland Zloty&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B120" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C120" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''RUB''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Russia Ruble&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="PYG"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Paraguay Guarani&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B121" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C121" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''RWF''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Rwanda Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="QAR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Qatar Riyal&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B122" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C122" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''SAR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Saudi Arabia Riyal&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="RON"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Romania New Leu&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B123" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="C123" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''SBD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Solomon Islands Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="RSD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Serbia Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B124" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C124" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''SCR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Seychelles Rupee&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="RUB"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Russia Ruble&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B125" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="C125" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''SDG''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Sudan Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="RWF"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Rwanda Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B126" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C126" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''SEK''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Sweden Krona&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="SAR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Saudi Arabia Riyal&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B127" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="C127" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''SGD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Singapore Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="SBD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Solomon Islands Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B128" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C128" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;xs:enumeration value=''SHP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Saint Helena Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="SCR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Seychelles Rupee&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B129" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C129" t="str">
-        <f t="shared" ref="C129:C164" si="2">CONCATENATE("&lt;xs:enumeration value=''",A129,"''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;",B129,"&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;")</f>
-        <v>&lt;xs:enumeration value=''SLL''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Sierra Leone Leone&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <f t="shared" si="1"/>
+        <v>&lt;xs:enumeration value="SDG"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Sudan Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B130" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C130" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''SOS''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Somalia Shilling&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <f t="shared" si="1"/>
+        <v>&lt;xs:enumeration value="SEK"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Sweden Krona&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="B131" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C131" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''SPL*''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Seborga Luigino&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <f t="shared" si="1"/>
+        <v>&lt;xs:enumeration value="SGD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Singapore Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B132" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C132" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''SRD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Suriname Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <f t="shared" si="1"/>
+        <v>&lt;xs:enumeration value="SHP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Saint Helena Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B133" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C133" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''STD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;São Tomé and Príncipe Dobra&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <f t="shared" si="1"/>
+        <v>&lt;xs:enumeration value="SLL"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Sierra Leone Leone&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B134" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C134" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''SVC''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;El Salvador Colon&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <f t="shared" ref="C134:C168" si="2">CONCATENATE("&lt;xs:enumeration value=""",A134,"""&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;",B134,"&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;")</f>
+        <v>&lt;xs:enumeration value="SOS"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Somalia Shilling&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B135" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C135" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''SYP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Syria Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="SPL*"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Seborga Luigino&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B136" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C136" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''SZL''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Swaziland Lilangeni&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="SRD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Suriname Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B137" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C137" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''THB''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Thailand Baht&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="STD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;São Tomé and Príncipe Dobra&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B138" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C138" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''TJS''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Tajikistan Somoni&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="SVC"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;El Salvador Colon&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B139" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C139" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''TMT''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Turkmenistan Manat&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="SYP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Syria Pound&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B140" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C140" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''TND''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Tunisia Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="SZL"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Swaziland Lilangeni&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B141" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C141" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''TOP''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Tonga Pa'anga&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="THB"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Thailand Baht&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B142" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C142" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''TRY''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Turkey Lira&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="TJS"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Tajikistan Somoni&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B143" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C143" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''TTD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Trinidad and Tobago Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="TMT"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Turkmenistan Manat&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B144" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C144" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''TVD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Tuvalu Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="TND"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Tunisia Dinar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B145" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="C145" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''TWD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Taiwan New Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="TOP"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Tonga Pa'anga&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B146" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="C146" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''TZS''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Tanzania Shilling&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="TRY"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Turkey Lira&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B147" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C147" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''UAH''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Ukraine Hryvna&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="TTD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Trinidad and Tobago Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B148" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="C148" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''UGX''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Uganda Shilling&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="TVD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Tuvalu Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B149" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C149" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''USD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;United States Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="TWD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Taiwan New Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B150" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="C150" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''UYU''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Uruguay Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="TZS"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Tanzania Shilling&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B151" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="C151" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''UZS''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Uzbekistan Som&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="UAH"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Ukraine Hryvna&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B152" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="C152" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''VEF''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Venezuela Bolivar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="UGX"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Uganda Shilling&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B153" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="C153" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''VND''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Viet Nam Dong&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="USD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;United States Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B154" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="C154" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''VUV''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Vanuatu Vatu&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="UYU"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Uruguay Peso&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B155" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C155" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''WST''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Samoa Tala&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="UZS"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Uzbekistan Som&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="B156" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="C156" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''XAF''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Communauté Financière Africaine (BEAC) CFA Franc BEAC&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="VEF"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Venezuela Bolivar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B157" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C157" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''XCD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;East Caribbean Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="VND"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Viet Nam Dong&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="B158" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="C158" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''XDR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;International Monetary Fund (IMF) Special Drawing Rights&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="VUV"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Vanuatu Vatu&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B159" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="C159" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''XOF''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Communauté Financière Africaine (BCEAO) Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="WST"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Samoa Tala&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B160" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="C160" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''XPF''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Comptoirs Français du Pacifique (CFP) Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="XAF"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Communauté Financière Africaine (BEAC) CFA Franc BEAC&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="B161" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C161" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''YER''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Yemen Rial&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="XCD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;East Caribbean Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="B162" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C162" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''ZAR''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;South Africa Rand&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="XDR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;International Monetary Fund (IMF) Special Drawing Rights&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B163" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C163" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''ZMW''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Zambia Kwacha&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="XOF"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Communauté Financière Africaine (BCEAO) Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B164" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="C164" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;xs:enumeration value=''ZWD''&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Zimbabwe Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+        <v>&lt;xs:enumeration value="XPF"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Comptoirs Français du Pacifique (CFP) Franc&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" t="s">
+        <v>320</v>
+      </c>
+      <c r="B165" t="s">
+        <v>321</v>
+      </c>
+      <c r="C165" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;xs:enumeration value="YER"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Yemen Rial&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" t="s">
+        <v>322</v>
+      </c>
+      <c r="B166" t="s">
+        <v>323</v>
+      </c>
+      <c r="C166" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;xs:enumeration value="ZAR"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;South Africa Rand&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" t="s">
+        <v>324</v>
+      </c>
+      <c r="B167" t="s">
+        <v>325</v>
+      </c>
+      <c r="C167" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;xs:enumeration value="ZMW"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Zambia Kwacha&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" t="s">
+        <v>326</v>
+      </c>
+      <c r="B168" t="s">
+        <v>327</v>
+      </c>
+      <c r="C168" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;xs:enumeration value="ZWD"&gt;&lt;xs:annotation&gt;&lt;xs:documentation&gt;Zimbabwe Dollar&lt;/xs:documentation&gt;&lt;/xs:annotation&gt;&lt;/xs:enumeration&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>